<commit_message>
BUFF_AA 구현 및 버프 Function을 위한 base 작성
- trivial : 마나 마커 삭제. 혹시 몰라 남겨는 놓음
- AI의 타겟팅을 위한 전략을 Projectile에서 분리. 작동 확인함
- FunctionData에 문제 있어 수정함
</commit_message>
<xml_diff>
--- a/DataGenerator/XLSXS/FunctionData.xlsx
+++ b/DataGenerator/XLSXS/FunctionData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\DG_Project\DataGenerator\XLSXS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jehee\Documents\GitHub\DG_Project\DataGenerator\XLSXS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D582D9-48EF-473D-A2A2-A7D7CABD8F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644D0D93-B612-41B7-A82E-05740863603E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7335" yWindow="735" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2265" yWindow="2625" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트8" sheetId="1" r:id="rId1"/>
@@ -375,7 +375,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[600711,600712]</t>
+    <t>[600711.600712]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -738,8 +738,8 @@
   </sheetPr>
   <dimension ref="A1:N127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -899,7 +899,9 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1">
+        <v>-1</v>
+      </c>
       <c r="I4" s="1">
         <v>2</v>
       </c>

</xml_diff>